<commit_message>
Minor updates to data_request file
</commit_message>
<xml_diff>
--- a/code_books/requested_data.xlsx
+++ b/code_books/requested_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skipmoses/Dropbox/Classwork/CurrentSemester/MATH485/consulting-project-SI/code_books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3851475-A620-644A-8006-CCC49291A74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F214B5-347B-F04F-9A8E-A05FB9E98FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12620" yWindow="1000" windowWidth="14400" windowHeight="13260" xr2:uid="{53956DD0-68DD-C84F-A616-80B4FE3A397C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Blinded student ID</t>
   </si>
@@ -157,18 +157,12 @@
     <t>Academic data –at time of graduation</t>
   </si>
   <si>
-    <t>Data set 2: Class level(one record per person-per classwhere SI was offered)</t>
-  </si>
-  <si>
     <t>At the time of taking class</t>
   </si>
   <si>
     <t xml:space="preserve">The semester prior to taking the class. </t>
   </si>
   <si>
-    <t>Data set 3:SI related data (one record per personper visit)</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -176,19 +170,41 @@
   </si>
   <si>
     <t>Grade in class(STDNT_CLASS_OFFCL_GRD)</t>
+  </si>
+  <si>
+    <t>Data set 2: Class level(one record per person-per 
+classwhere SI was offered)</t>
+  </si>
+  <si>
+    <t>Data set 3:SI related data (one record per
+ personper visit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,8 +227,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,11 +548,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E916C9-2A61-5640-A12F-772FBF7C5920}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -543,43 +562,29 @@
     <col min="11" max="11" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="E3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -587,66 +592,57 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -654,29 +650,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -684,7 +680,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -692,7 +688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -700,17 +696,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -718,20 +714,26 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
-        <v>42</v>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -740,7 +742,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C21" t="s">
@@ -752,7 +754,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -762,18 +764,24 @@
       <c r="A23" t="s">
         <v>15</v>
       </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
slight edit to data request
</commit_message>
<xml_diff>
--- a/code_books/requested_data.xlsx
+++ b/code_books/requested_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skipmoses/Dropbox/Classwork/CurrentSemester/MATH485/consulting-project-SI/code_books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\DATA485\consulting-project-si-1\code_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F214B5-347B-F04F-9A8E-A05FB9E98FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B51895B-C383-424C-99D9-E5BBC8404D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="1000" windowWidth="14400" windowHeight="13260" xr2:uid="{53956DD0-68DD-C84F-A616-80B4FE3A397C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53956DD0-68DD-C84F-A616-80B4FE3A397C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Blinded student ID</t>
   </si>
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -548,11 +548,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E916C9-2A61-5640-A12F-772FBF7C5920}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="54.33203125" customWidth="1"/>
     <col min="3" max="3" width="77.33203125" customWidth="1"/>
@@ -562,7 +564,7 @@
     <col min="11" max="11" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="60">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -573,7 +575,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -583,8 +585,11 @@
       <c r="E3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -594,8 +599,11 @@
       <c r="E4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -608,8 +616,11 @@
       <c r="E5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -622,8 +633,11 @@
       <c r="E6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -631,7 +645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -642,7 +656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -650,7 +664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -661,7 +675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -672,7 +686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -680,7 +694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -688,7 +702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -696,12 +710,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="C15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -709,15 +723,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
       <c r="C17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -725,7 +742,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -736,12 +753,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="C20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -749,7 +766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -760,7 +777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -768,7 +785,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -776,7 +793,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -784,7 +801,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>18</v>
       </c>

</xml_diff>